<commit_message>
order list voor sjriek
</commit_message>
<xml_diff>
--- a/Documentation/Order list voor Sjriek.xlsx
+++ b/Documentation/Order list voor Sjriek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Orderlist</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Total costs</t>
+  </si>
+  <si>
+    <t>Lazy Susan</t>
+  </si>
+  <si>
+    <t>Bylim</t>
+  </si>
+  <si>
+    <t>Kingduino</t>
+  </si>
+  <si>
+    <t>https://hobbyking.com/nl_nl/kingduino-atmel-atmega-328-pu.html</t>
   </si>
 </sst>
 </file>
@@ -248,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -258,6 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -573,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +652,7 @@
         <v>16.95</v>
       </c>
       <c r="F5" s="6">
-        <f>SUM(D5*E5)</f>
+        <f t="shared" ref="F5:F11" si="0">SUM(D5*E5)</f>
         <v>50.849999999999994</v>
       </c>
     </row>
@@ -660,7 +673,7 @@
         <v>13.95</v>
       </c>
       <c r="F6" s="6">
-        <f>SUM(D6*E6)</f>
+        <f t="shared" si="0"/>
         <v>41.849999999999994</v>
       </c>
     </row>
@@ -668,14 +681,22 @@
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4">
+        <v>7.81</v>
+      </c>
       <c r="F7" s="6">
-        <f>SUM(D7*E7)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>23.43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -693,7 +714,7 @@
         <v>2.38</v>
       </c>
       <c r="F8" s="6">
-        <f>SUM(D8*E8)</f>
+        <f t="shared" si="0"/>
         <v>7.14</v>
       </c>
       <c r="H8" t="s">
@@ -715,7 +736,7 @@
         <v>16.95</v>
       </c>
       <c r="F9" s="6">
-        <f>SUM(D9*E9)</f>
+        <f t="shared" si="0"/>
         <v>50.849999999999994</v>
       </c>
       <c r="H9" t="s">
@@ -739,7 +760,7 @@
         <v>2.99</v>
       </c>
       <c r="F10" s="4">
-        <f>SUM(D10*E10)</f>
+        <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
     </row>
@@ -760,7 +781,7 @@
         <v>7.38</v>
       </c>
       <c r="F11" s="4">
-        <f>SUM(D11*E11)</f>
+        <f t="shared" si="0"/>
         <v>7.38</v>
       </c>
     </row>
@@ -804,7 +825,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6">
+        <f>SUM(D16*E16)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -856,15 +880,34 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
+      <c r="F19" s="6">
+        <f>SUM(D19*E19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
         <v>36</v>
       </c>
-      <c r="F21">
-        <f>SUM(F5:F19)</f>
-        <v>175.07</v>
+      <c r="F22">
+        <f>SUM(F5:F20)</f>
+        <v>263.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>